<commit_message>
Futher runs and comparisons
</commit_message>
<xml_diff>
--- a/Data/Model Comparisons/Model_Comparisons_v1.xlsx
+++ b/Data/Model Comparisons/Model_Comparisons_v1.xlsx
@@ -8,14 +8,16 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/stuartgow/GitHub/EEG_ML_Pipeline/Data/Model Comparisons/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E0485582-FABC-A44C-BD2B-762522806140}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DDCAEDC9-E56A-1C4E-B56D-69A71A73005F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="21880" yWindow="620" windowWidth="29320" windowHeight="26020" xr2:uid="{4EF99E70-5403-6B47-9FEC-848AE0CD045D}"/>
+    <workbookView xWindow="25400" yWindow="3040" windowWidth="27880" windowHeight="16940" xr2:uid="{72FD3ABC-35F6-DD46-8E40-52D9FE6A99D2}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Conclusions" sheetId="4" r:id="rId1"/>
+    <sheet name="First Runs" sheetId="1" r:id="rId2"/>
+    <sheet name="Extract" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -36,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="299" uniqueCount="108">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="464" uniqueCount="152">
   <si>
     <t>Model</t>
   </si>
@@ -363,6 +365,139 @@
   </si>
   <si>
     <t>Very good TP but several FN</t>
+  </si>
+  <si>
+    <t>IOWA_Rest</t>
+  </si>
+  <si>
+    <t>('2_Feature_Selection_Training_Run_20250812_search_periodic_channel',)</t>
+  </si>
+  <si>
+    <t>(['channel'],)</t>
+  </si>
+  <si>
+    <t>([['cf', 'pw', 'bw']],)</t>
+  </si>
+  <si>
+    <t>{'classifier__criterion': 'entropy', 'classifier__max_depth': 10, 'classifier__max_leaf_nodes': None, 'classifier__n_estimators': 150, 'features_selection__features_detail_level': 'channel', 'features_selection__selected_features': ['cf', 'pw', 'bw']}</t>
+  </si>
+  <si>
+    <t>channel</t>
+  </si>
+  <si>
+    <t>['cf', 'pw', 'bw']</t>
+  </si>
+  <si>
+    <t>RandomForest_v1</t>
+  </si>
+  <si>
+    <t>('2_Feature_Selection_Training_Run_20250813_search_subgroups',)</t>
+  </si>
+  <si>
+    <t>(['region', 'channel'],)</t>
+  </si>
+  <si>
+    <t>([['exp', 'offset'], ['cf', 'pw', 'bw'], ['age', 'gender']],)</t>
+  </si>
+  <si>
+    <t>{'classifier__activation': 'tanh', 'classifier__alpha': 0.1, 'classifier__batch_size': 'auto', 'classifier__hidden_layer_sizes': (50, 50), 'classifier__learning_rate_init': 0.001, 'classifier__max_iter': 1000, 'classifier__solver': 'adam', 'features_selection__features_detail_level': 'channel', 'features_selection__selected_features': ['exp', 'offset']}</t>
+  </si>
+  <si>
+    <t>['exp', 'offset']</t>
+  </si>
+  <si>
+    <t>MLPClassifier_v1</t>
+  </si>
+  <si>
+    <t>{'classifier__C': 1, 'classifier__class_weight': 'balanced', 'classifier__max_iter': 1000, 'classifier__penalty': 'l1', 'classifier__solver': 'liblinear', 'features_selection__features_detail_level': 'channel', 'features_selection__selected_features': ['cf', 'pw', 'bw']}</t>
+  </si>
+  <si>
+    <t>LogisticRegression_v1</t>
+  </si>
+  <si>
+    <t>study</t>
+  </si>
+  <si>
+    <t>training_source_data_run</t>
+  </si>
+  <si>
+    <t>training_results_run</t>
+  </si>
+  <si>
+    <t>search_features_detail</t>
+  </si>
+  <si>
+    <t>search_features_selection</t>
+  </si>
+  <si>
+    <t>CV_search_time</t>
+  </si>
+  <si>
+    <t>CV_best_parameters</t>
+  </si>
+  <si>
+    <t>features_detail</t>
+  </si>
+  <si>
+    <t>features_selection</t>
+  </si>
+  <si>
+    <t>model_name</t>
+  </si>
+  <si>
+    <t>prediction_time</t>
+  </si>
+  <si>
+    <t>mcc</t>
+  </si>
+  <si>
+    <t>recall</t>
+  </si>
+  <si>
+    <t>precision</t>
+  </si>
+  <si>
+    <t>f1_score</t>
+  </si>
+  <si>
+    <t>specificity</t>
+  </si>
+  <si>
+    <t>('2_Feature_Selection_Training_Run_20250812_search_periodic_region',)</t>
+  </si>
+  <si>
+    <t>(['region'],)</t>
+  </si>
+  <si>
+    <t>{'classifier__criterion': 'entropy', 'classifier__max_depth': 10, 'classifier__max_leaf_nodes': 50, 'classifier__n_estimators': 150, 'features_selection__features_detail_level': 'region', 'features_selection__selected_features': ['cf', 'pw', 'bw']}</t>
+  </si>
+  <si>
+    <t>region</t>
+  </si>
+  <si>
+    <t>('2_Feature_Selection_Training_Run_20250813_search_aperiodic_region',)</t>
+  </si>
+  <si>
+    <t>([['exp', 'offset']],)</t>
+  </si>
+  <si>
+    <t>{'classifier__activation': 'relu', 'classifier__alpha': 0.1, 'classifier__batch_size': 'auto', 'classifier__hidden_layer_sizes': (50, 50), 'classifier__learning_rate_init': 0.0001, 'classifier__max_iter': 1000, 'classifier__solver': 'adam', 'features_selection__features_detail_level': 'region', 'features_selection__selected_features': ['exp', 'offset']}</t>
+  </si>
+  <si>
+    <t>{'classifier__C': 10, 'classifier__class_weight': None, 'classifier__max_iter': 1000, 'classifier__penalty': 'l1', 'classifier__solver': 'liblinear', 'features_selection__features_detail_level': 'region', 'features_selection__selected_features': ['cf', 'pw', 'bw']}</t>
+  </si>
+  <si>
+    <t>Top Two Models Per Model Type</t>
+  </si>
+  <si>
+    <t>Aperiodic</t>
+  </si>
+  <si>
+    <t>››</t>
+  </si>
+  <si>
+    <t>Run 
+Time</t>
   </si>
 </sst>
 </file>
@@ -407,7 +542,7 @@
       <family val="2"/>
     </font>
   </fonts>
-  <fills count="8">
+  <fills count="9">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -450,8 +585,14 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="3" tint="0.749992370372631"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="10">
+  <borders count="12">
     <border>
       <left/>
       <right/>
@@ -558,11 +699,29 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="37">
+  <cellXfs count="58">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center"/>
@@ -631,31 +790,92 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="0" fillId="3" borderId="7" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="3" borderId="2" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="3" borderId="6" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="8" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="8" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="8" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="8" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="8" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -996,11 +1216,695 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{18C4033D-58B5-094F-86A4-FB568BC9D1B8}">
+  <dimension ref="A1:AB27"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="K8" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
+      <selection activeCell="U28" sqref="U28"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="1.83203125" customWidth="1"/>
+    <col min="2" max="2" width="11.1640625" customWidth="1"/>
+    <col min="3" max="3" width="6.6640625" customWidth="1"/>
+    <col min="8" max="8" width="14" customWidth="1"/>
+    <col min="10" max="10" width="16" customWidth="1"/>
+    <col min="11" max="11" width="17.1640625" customWidth="1"/>
+    <col min="18" max="18" width="2" customWidth="1"/>
+    <col min="19" max="19" width="2.33203125" customWidth="1"/>
+    <col min="20" max="20" width="17.83203125" customWidth="1"/>
+    <col min="28" max="28" width="2.6640625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:28" x14ac:dyDescent="0.2">
+      <c r="A1" s="8" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="3" spans="1:28" s="37" customFormat="1" ht="68" x14ac:dyDescent="0.2">
+      <c r="B3" s="38" t="s">
+        <v>124</v>
+      </c>
+      <c r="C3" s="38" t="s">
+        <v>125</v>
+      </c>
+      <c r="D3" s="38" t="s">
+        <v>126</v>
+      </c>
+      <c r="E3" s="38" t="s">
+        <v>127</v>
+      </c>
+      <c r="F3" s="38" t="s">
+        <v>128</v>
+      </c>
+      <c r="G3" s="38" t="s">
+        <v>129</v>
+      </c>
+      <c r="H3" s="38" t="s">
+        <v>130</v>
+      </c>
+      <c r="I3" s="38" t="s">
+        <v>131</v>
+      </c>
+      <c r="J3" s="38" t="s">
+        <v>132</v>
+      </c>
+      <c r="K3" s="38" t="s">
+        <v>133</v>
+      </c>
+      <c r="L3" s="38" t="s">
+        <v>134</v>
+      </c>
+      <c r="M3" s="38" t="s">
+        <v>135</v>
+      </c>
+      <c r="N3" s="38" t="s">
+        <v>136</v>
+      </c>
+      <c r="O3" s="38" t="s">
+        <v>137</v>
+      </c>
+      <c r="P3" s="38" t="s">
+        <v>138</v>
+      </c>
+      <c r="Q3" s="38" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="5" spans="1:28" s="50" customFormat="1" ht="61" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A5" s="50">
+        <v>3</v>
+      </c>
+      <c r="B5" s="50" t="s">
+        <v>108</v>
+      </c>
+      <c r="C5" s="50" t="s">
+        <v>19</v>
+      </c>
+      <c r="D5" s="50" t="s">
+        <v>109</v>
+      </c>
+      <c r="E5" s="50" t="s">
+        <v>110</v>
+      </c>
+      <c r="F5" s="50" t="s">
+        <v>111</v>
+      </c>
+      <c r="G5" s="50">
+        <v>9.4758856249973107</v>
+      </c>
+      <c r="H5" s="51" t="s">
+        <v>112</v>
+      </c>
+      <c r="I5" s="50" t="s">
+        <v>113</v>
+      </c>
+      <c r="J5" s="50" t="s">
+        <v>114</v>
+      </c>
+      <c r="K5" s="50" t="s">
+        <v>115</v>
+      </c>
+      <c r="L5" s="50">
+        <v>6.2812416988890604E-2</v>
+      </c>
+      <c r="M5" s="50">
+        <v>0.56937799043062198</v>
+      </c>
+      <c r="N5" s="50">
+        <v>0.84210526315789402</v>
+      </c>
+      <c r="O5" s="50">
+        <v>0.84210526315789402</v>
+      </c>
+      <c r="P5" s="50">
+        <v>0.84210526315789402</v>
+      </c>
+      <c r="Q5" s="50">
+        <v>0.72727272727272696</v>
+      </c>
+    </row>
+    <row r="6" spans="1:28" s="50" customFormat="1" ht="61" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A6" s="50">
+        <v>0</v>
+      </c>
+      <c r="B6" s="50" t="s">
+        <v>108</v>
+      </c>
+      <c r="C6" s="50" t="s">
+        <v>19</v>
+      </c>
+      <c r="D6" s="50" t="s">
+        <v>140</v>
+      </c>
+      <c r="E6" s="50" t="s">
+        <v>141</v>
+      </c>
+      <c r="F6" s="50" t="s">
+        <v>111</v>
+      </c>
+      <c r="G6" s="50">
+        <v>7.8896797919878701</v>
+      </c>
+      <c r="H6" s="51" t="s">
+        <v>142</v>
+      </c>
+      <c r="I6" s="50" t="s">
+        <v>143</v>
+      </c>
+      <c r="J6" s="50" t="s">
+        <v>114</v>
+      </c>
+      <c r="K6" s="50" t="s">
+        <v>115</v>
+      </c>
+      <c r="L6" s="50">
+        <v>5.3513499995460699E-2</v>
+      </c>
+      <c r="M6" s="50">
+        <v>0.43808582711518002</v>
+      </c>
+      <c r="N6" s="50">
+        <v>1</v>
+      </c>
+      <c r="O6" s="50">
+        <v>0.70370370370370305</v>
+      </c>
+      <c r="P6" s="50">
+        <v>0.82608695652173902</v>
+      </c>
+      <c r="Q6" s="50">
+        <v>0.27272727272727199</v>
+      </c>
+    </row>
+    <row r="7" spans="1:28" s="50" customFormat="1" ht="61" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A7" s="50">
+        <v>11</v>
+      </c>
+      <c r="B7" s="50" t="s">
+        <v>108</v>
+      </c>
+      <c r="C7" s="50" t="s">
+        <v>19</v>
+      </c>
+      <c r="D7" s="50" t="s">
+        <v>116</v>
+      </c>
+      <c r="E7" s="50" t="s">
+        <v>117</v>
+      </c>
+      <c r="F7" s="50" t="s">
+        <v>118</v>
+      </c>
+      <c r="G7" s="50">
+        <v>30.170736916013901</v>
+      </c>
+      <c r="H7" s="51" t="s">
+        <v>119</v>
+      </c>
+      <c r="I7" s="50" t="s">
+        <v>113</v>
+      </c>
+      <c r="J7" s="50" t="s">
+        <v>120</v>
+      </c>
+      <c r="K7" s="50" t="s">
+        <v>121</v>
+      </c>
+      <c r="L7" s="50">
+        <v>6.3386250112671396E-3</v>
+      </c>
+      <c r="M7" s="50">
+        <v>0.39795757799683601</v>
+      </c>
+      <c r="N7" s="50">
+        <v>0.89473684210526305</v>
+      </c>
+      <c r="O7" s="50">
+        <v>0.73913043478260798</v>
+      </c>
+      <c r="P7" s="50">
+        <v>0.80952380952380898</v>
+      </c>
+      <c r="Q7" s="50">
+        <v>0.45454545454545398</v>
+      </c>
+    </row>
+    <row r="8" spans="1:28" s="50" customFormat="1" ht="61" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A8" s="50">
+        <v>17</v>
+      </c>
+      <c r="B8" s="50" t="s">
+        <v>108</v>
+      </c>
+      <c r="C8" s="50" t="s">
+        <v>19</v>
+      </c>
+      <c r="D8" s="50" t="s">
+        <v>144</v>
+      </c>
+      <c r="E8" s="50" t="s">
+        <v>141</v>
+      </c>
+      <c r="F8" s="50" t="s">
+        <v>145</v>
+      </c>
+      <c r="G8" s="50">
+        <v>2.5997217079857302</v>
+      </c>
+      <c r="H8" s="51" t="s">
+        <v>146</v>
+      </c>
+      <c r="I8" s="50" t="s">
+        <v>143</v>
+      </c>
+      <c r="J8" s="50" t="s">
+        <v>120</v>
+      </c>
+      <c r="K8" s="50" t="s">
+        <v>121</v>
+      </c>
+      <c r="L8" s="50">
+        <v>3.7227499997243198E-3</v>
+      </c>
+      <c r="M8" s="50">
+        <v>0.20751433915982201</v>
+      </c>
+      <c r="N8" s="50">
+        <v>0.94736842105263097</v>
+      </c>
+      <c r="O8" s="50">
+        <v>0.66666666666666596</v>
+      </c>
+      <c r="P8" s="50">
+        <v>0.78260869565217395</v>
+      </c>
+      <c r="Q8" s="50">
+        <v>0.18181818181818099</v>
+      </c>
+    </row>
+    <row r="9" spans="1:28" s="50" customFormat="1" ht="61" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A9" s="50">
+        <v>4</v>
+      </c>
+      <c r="B9" s="50" t="s">
+        <v>108</v>
+      </c>
+      <c r="C9" s="50" t="s">
+        <v>19</v>
+      </c>
+      <c r="D9" s="50" t="s">
+        <v>109</v>
+      </c>
+      <c r="E9" s="50" t="s">
+        <v>110</v>
+      </c>
+      <c r="F9" s="50" t="s">
+        <v>111</v>
+      </c>
+      <c r="G9" s="50">
+        <v>68.521575916005503</v>
+      </c>
+      <c r="H9" s="51" t="s">
+        <v>122</v>
+      </c>
+      <c r="I9" s="50" t="s">
+        <v>113</v>
+      </c>
+      <c r="J9" s="50" t="s">
+        <v>114</v>
+      </c>
+      <c r="K9" s="50" t="s">
+        <v>123</v>
+      </c>
+      <c r="L9" s="50">
+        <v>1.2745333020575299E-2</v>
+      </c>
+      <c r="M9" s="50">
+        <v>0.29578954665861401</v>
+      </c>
+      <c r="N9" s="50">
+        <v>0.57894736842105199</v>
+      </c>
+      <c r="O9" s="50">
+        <v>0.78571428571428503</v>
+      </c>
+      <c r="P9" s="50">
+        <v>0.66666666666666596</v>
+      </c>
+      <c r="Q9" s="50">
+        <v>0.72727272727272696</v>
+      </c>
+    </row>
+    <row r="10" spans="1:28" s="50" customFormat="1" ht="61" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A10" s="50">
+        <v>1</v>
+      </c>
+      <c r="B10" s="50" t="s">
+        <v>108</v>
+      </c>
+      <c r="C10" s="50" t="s">
+        <v>19</v>
+      </c>
+      <c r="D10" s="50" t="s">
+        <v>140</v>
+      </c>
+      <c r="E10" s="50" t="s">
+        <v>141</v>
+      </c>
+      <c r="F10" s="50" t="s">
+        <v>111</v>
+      </c>
+      <c r="G10" s="50">
+        <v>4.7643824999977298</v>
+      </c>
+      <c r="H10" s="51" t="s">
+        <v>147</v>
+      </c>
+      <c r="I10" s="50" t="s">
+        <v>143</v>
+      </c>
+      <c r="J10" s="50" t="s">
+        <v>114</v>
+      </c>
+      <c r="K10" s="50" t="s">
+        <v>123</v>
+      </c>
+      <c r="L10" s="50">
+        <v>8.1201082997722496E-2</v>
+      </c>
+      <c r="M10" s="50">
+        <v>0.23441336786115</v>
+      </c>
+      <c r="N10" s="50">
+        <v>0.84210526315789402</v>
+      </c>
+      <c r="O10" s="50">
+        <v>0.69565217391304301</v>
+      </c>
+      <c r="P10" s="50">
+        <v>0.76190476190476097</v>
+      </c>
+      <c r="Q10" s="50">
+        <v>0.36363636363636298</v>
+      </c>
+    </row>
+    <row r="11" spans="1:28" ht="19" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="12" spans="1:28" x14ac:dyDescent="0.2">
+      <c r="S12" s="6"/>
+      <c r="T12" s="6"/>
+      <c r="U12" s="6"/>
+      <c r="V12" s="6"/>
+      <c r="W12" s="6"/>
+      <c r="X12" s="6"/>
+      <c r="Y12" s="6"/>
+      <c r="Z12" s="6"/>
+      <c r="AA12" s="6"/>
+      <c r="AB12" s="6"/>
+    </row>
+    <row r="13" spans="1:28" x14ac:dyDescent="0.2">
+      <c r="S13" s="6"/>
+      <c r="T13" s="34" t="s">
+        <v>0</v>
+      </c>
+      <c r="U13" s="47" t="s">
+        <v>14</v>
+      </c>
+      <c r="V13" s="47" t="s">
+        <v>13</v>
+      </c>
+      <c r="W13" s="36" t="s">
+        <v>151</v>
+      </c>
+      <c r="X13" s="56" t="s">
+        <v>5</v>
+      </c>
+      <c r="Y13" s="49" t="s">
+        <v>1</v>
+      </c>
+      <c r="Z13" s="49" t="s">
+        <v>2</v>
+      </c>
+      <c r="AA13" s="49" t="s">
+        <v>4</v>
+      </c>
+      <c r="AB13" s="6"/>
+    </row>
+    <row r="14" spans="1:28" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="S14" s="6"/>
+      <c r="T14" s="40"/>
+      <c r="U14" s="48"/>
+      <c r="V14" s="48"/>
+      <c r="W14" s="31"/>
+      <c r="X14" s="57"/>
+      <c r="Y14" s="48"/>
+      <c r="Z14" s="48"/>
+      <c r="AA14" s="48"/>
+      <c r="AB14" s="6"/>
+    </row>
+    <row r="15" spans="1:28" x14ac:dyDescent="0.2">
+      <c r="S15" s="6"/>
+      <c r="T15" s="52" t="s">
+        <v>6</v>
+      </c>
+      <c r="U15" s="42" t="s">
+        <v>10</v>
+      </c>
+      <c r="V15" s="43" t="s">
+        <v>52</v>
+      </c>
+      <c r="W15" s="44">
+        <f>L5</f>
+        <v>6.2812416988890604E-2</v>
+      </c>
+      <c r="X15" s="44">
+        <f>M5</f>
+        <v>0.56937799043062198</v>
+      </c>
+      <c r="Y15" s="44">
+        <f>N5</f>
+        <v>0.84210526315789402</v>
+      </c>
+      <c r="Z15" s="44">
+        <f>O5</f>
+        <v>0.84210526315789402</v>
+      </c>
+      <c r="AA15" s="44">
+        <f>Q5</f>
+        <v>0.72727272727272696</v>
+      </c>
+      <c r="AB15" s="6"/>
+    </row>
+    <row r="16" spans="1:28" ht="23" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="S16" s="6"/>
+      <c r="T16" s="53"/>
+      <c r="U16" s="39" t="s">
+        <v>26</v>
+      </c>
+      <c r="V16" s="12" t="s">
+        <v>52</v>
+      </c>
+      <c r="W16" s="2">
+        <f>L6</f>
+        <v>5.3513499995460699E-2</v>
+      </c>
+      <c r="X16" s="2">
+        <f>M6</f>
+        <v>0.43808582711518002</v>
+      </c>
+      <c r="Y16" s="2">
+        <f>N6</f>
+        <v>1</v>
+      </c>
+      <c r="Z16" s="2">
+        <f>O6</f>
+        <v>0.70370370370370305</v>
+      </c>
+      <c r="AA16" s="2">
+        <f>Q6</f>
+        <v>0.27272727272727199</v>
+      </c>
+      <c r="AB16" s="6"/>
+    </row>
+    <row r="17" spans="19:28" ht="23" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="S17" s="6"/>
+      <c r="T17" s="52" t="s">
+        <v>8</v>
+      </c>
+      <c r="U17" s="42" t="s">
+        <v>10</v>
+      </c>
+      <c r="V17" s="43" t="s">
+        <v>149</v>
+      </c>
+      <c r="W17" s="44">
+        <f>L7</f>
+        <v>6.3386250112671396E-3</v>
+      </c>
+      <c r="X17" s="44">
+        <f>M7</f>
+        <v>0.39795757799683601</v>
+      </c>
+      <c r="Y17" s="44">
+        <f>N7</f>
+        <v>0.89473684210526305</v>
+      </c>
+      <c r="Z17" s="44">
+        <f>O7</f>
+        <v>0.73913043478260798</v>
+      </c>
+      <c r="AA17" s="45">
+        <f>Q7</f>
+        <v>0.45454545454545398</v>
+      </c>
+      <c r="AB17" s="6"/>
+    </row>
+    <row r="18" spans="19:28" ht="23" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="S18" s="6"/>
+      <c r="T18" s="54"/>
+      <c r="U18" s="39" t="s">
+        <v>26</v>
+      </c>
+      <c r="V18" s="12" t="s">
+        <v>149</v>
+      </c>
+      <c r="W18" s="4">
+        <f>L8</f>
+        <v>3.7227499997243198E-3</v>
+      </c>
+      <c r="X18" s="4">
+        <f>M8</f>
+        <v>0.20751433915982201</v>
+      </c>
+      <c r="Y18" s="4">
+        <f>N8</f>
+        <v>0.94736842105263097</v>
+      </c>
+      <c r="Z18" s="4">
+        <f>O8</f>
+        <v>0.66666666666666596</v>
+      </c>
+      <c r="AA18" s="46">
+        <f>Q8</f>
+        <v>0.18181818181818099</v>
+      </c>
+      <c r="AB18" s="6"/>
+    </row>
+    <row r="19" spans="19:28" ht="23" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="S19" s="6"/>
+      <c r="T19" s="55" t="s">
+        <v>7</v>
+      </c>
+      <c r="U19" s="42" t="s">
+        <v>10</v>
+      </c>
+      <c r="V19" s="43" t="s">
+        <v>52</v>
+      </c>
+      <c r="W19" s="44">
+        <f>L9</f>
+        <v>1.2745333020575299E-2</v>
+      </c>
+      <c r="X19" s="44">
+        <f>M9</f>
+        <v>0.29578954665861401</v>
+      </c>
+      <c r="Y19" s="44">
+        <f>N9</f>
+        <v>0.57894736842105199</v>
+      </c>
+      <c r="Z19" s="44">
+        <f>O9</f>
+        <v>0.78571428571428503</v>
+      </c>
+      <c r="AA19" s="44">
+        <f>Q9</f>
+        <v>0.72727272727272696</v>
+      </c>
+      <c r="AB19" s="6"/>
+    </row>
+    <row r="20" spans="19:28" ht="23" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="S20" s="6"/>
+      <c r="T20" s="41"/>
+      <c r="U20" s="39" t="s">
+        <v>26</v>
+      </c>
+      <c r="V20" s="12" t="s">
+        <v>52</v>
+      </c>
+      <c r="W20" s="4">
+        <f>L10</f>
+        <v>8.1201082997722496E-2</v>
+      </c>
+      <c r="X20" s="4">
+        <f>M10</f>
+        <v>0.23441336786115</v>
+      </c>
+      <c r="Y20" s="4">
+        <f>N10</f>
+        <v>0.84210526315789402</v>
+      </c>
+      <c r="Z20" s="4">
+        <f>O10</f>
+        <v>0.69565217391304301</v>
+      </c>
+      <c r="AA20" s="4">
+        <f>Q10</f>
+        <v>0.36363636363636298</v>
+      </c>
+      <c r="AB20" s="6"/>
+    </row>
+    <row r="21" spans="19:28" x14ac:dyDescent="0.2">
+      <c r="S21" s="6"/>
+      <c r="T21" s="6"/>
+      <c r="U21" s="6"/>
+      <c r="V21" s="6"/>
+      <c r="W21" s="6"/>
+      <c r="X21" s="6"/>
+      <c r="Y21" s="6"/>
+      <c r="Z21" s="6"/>
+      <c r="AA21" s="6"/>
+      <c r="AB21" s="6"/>
+    </row>
+    <row r="22" spans="19:28" ht="8" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="S22" s="6"/>
+      <c r="T22" s="6"/>
+      <c r="U22" s="6"/>
+      <c r="V22" s="6"/>
+      <c r="W22" s="6"/>
+      <c r="X22" s="6"/>
+      <c r="Y22" s="6"/>
+      <c r="Z22" s="6"/>
+      <c r="AA22" s="6"/>
+      <c r="AB22" s="6"/>
+    </row>
+    <row r="27" spans="19:28" x14ac:dyDescent="0.2">
+      <c r="X27" t="s">
+        <v>150</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="8">
+    <mergeCell ref="Z13:Z14"/>
+    <mergeCell ref="AA13:AA14"/>
+    <mergeCell ref="T13:T14"/>
+    <mergeCell ref="U13:U14"/>
+    <mergeCell ref="V13:V14"/>
+    <mergeCell ref="W13:W14"/>
+    <mergeCell ref="X13:X14"/>
+    <mergeCell ref="Y13:Y14"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{87625442-3BD6-D848-B867-F3AC6454CEE0}">
   <dimension ref="A1:U144"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A18" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="I30" sqref="I30"/>
+    <sheetView topLeftCell="A28" workbookViewId="0">
+      <selection activeCell="M20" sqref="M20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1039,46 +1943,46 @@
     </row>
     <row r="4" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A4" s="6"/>
-      <c r="B4" s="32" t="s">
+      <c r="B4" s="34" t="s">
         <v>0</v>
       </c>
-      <c r="C4" s="30" t="s">
+      <c r="C4" s="36" t="s">
         <v>14</v>
       </c>
-      <c r="D4" s="30" t="s">
+      <c r="D4" s="36" t="s">
         <v>13</v>
       </c>
-      <c r="E4" s="30" t="s">
+      <c r="E4" s="36" t="s">
         <v>12</v>
       </c>
-      <c r="F4" s="34" t="s">
+      <c r="F4" s="30" t="s">
         <v>1</v>
       </c>
-      <c r="G4" s="35" t="s">
+      <c r="G4" s="28" t="s">
         <v>2</v>
       </c>
-      <c r="H4" s="34" t="s">
+      <c r="H4" s="30" t="s">
         <v>3</v>
       </c>
-      <c r="I4" s="34" t="s">
+      <c r="I4" s="30" t="s">
         <v>4</v>
       </c>
-      <c r="J4" s="28" t="s">
+      <c r="J4" s="32" t="s">
         <v>5</v>
       </c>
       <c r="K4" s="6"/>
     </row>
     <row r="5" spans="1:13" ht="19" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5" s="6"/>
-      <c r="B5" s="33"/>
+      <c r="B5" s="35"/>
       <c r="C5" s="31"/>
       <c r="D5" s="31"/>
       <c r="E5" s="31"/>
       <c r="F5" s="31"/>
-      <c r="G5" s="36"/>
+      <c r="G5" s="29"/>
       <c r="H5" s="31"/>
       <c r="I5" s="31"/>
-      <c r="J5" s="29"/>
+      <c r="J5" s="33"/>
       <c r="K5" s="6"/>
     </row>
     <row r="6" spans="1:13" s="1" customFormat="1" ht="24" customHeight="1" x14ac:dyDescent="0.2">
@@ -1273,46 +2177,46 @@
     </row>
     <row r="21" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A21" s="6"/>
-      <c r="B21" s="32" t="s">
+      <c r="B21" s="34" t="s">
         <v>0</v>
       </c>
-      <c r="C21" s="30" t="s">
+      <c r="C21" s="36" t="s">
         <v>14</v>
       </c>
-      <c r="D21" s="30" t="s">
+      <c r="D21" s="36" t="s">
         <v>13</v>
       </c>
-      <c r="E21" s="30" t="s">
+      <c r="E21" s="36" t="s">
         <v>12</v>
       </c>
-      <c r="F21" s="34" t="s">
+      <c r="F21" s="30" t="s">
         <v>1</v>
       </c>
-      <c r="G21" s="35" t="s">
+      <c r="G21" s="28" t="s">
         <v>2</v>
       </c>
-      <c r="H21" s="34" t="s">
+      <c r="H21" s="30" t="s">
         <v>3</v>
       </c>
-      <c r="I21" s="34" t="s">
+      <c r="I21" s="30" t="s">
         <v>4</v>
       </c>
-      <c r="J21" s="28" t="s">
+      <c r="J21" s="32" t="s">
         <v>5</v>
       </c>
       <c r="K21" s="6"/>
     </row>
     <row r="22" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A22" s="6"/>
-      <c r="B22" s="33"/>
+      <c r="B22" s="35"/>
       <c r="C22" s="31"/>
       <c r="D22" s="31"/>
       <c r="E22" s="31"/>
       <c r="F22" s="31"/>
-      <c r="G22" s="36"/>
+      <c r="G22" s="29"/>
       <c r="H22" s="31"/>
       <c r="I22" s="31"/>
-      <c r="J22" s="29"/>
+      <c r="J22" s="33"/>
       <c r="K22" s="6"/>
     </row>
     <row r="23" spans="1:16" ht="28" customHeight="1" x14ac:dyDescent="0.2">
@@ -1509,46 +2413,46 @@
     </row>
     <row r="37" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A37" s="6"/>
-      <c r="B37" s="32" t="s">
+      <c r="B37" s="34" t="s">
         <v>0</v>
       </c>
-      <c r="C37" s="30" t="s">
+      <c r="C37" s="36" t="s">
         <v>14</v>
       </c>
-      <c r="D37" s="30" t="s">
+      <c r="D37" s="36" t="s">
         <v>13</v>
       </c>
-      <c r="E37" s="30" t="s">
+      <c r="E37" s="36" t="s">
         <v>12</v>
       </c>
-      <c r="F37" s="34" t="s">
+      <c r="F37" s="30" t="s">
         <v>1</v>
       </c>
-      <c r="G37" s="35" t="s">
+      <c r="G37" s="28" t="s">
         <v>2</v>
       </c>
-      <c r="H37" s="34" t="s">
+      <c r="H37" s="30" t="s">
         <v>3</v>
       </c>
-      <c r="I37" s="34" t="s">
+      <c r="I37" s="30" t="s">
         <v>4</v>
       </c>
-      <c r="J37" s="28" t="s">
+      <c r="J37" s="32" t="s">
         <v>5</v>
       </c>
       <c r="K37" s="6"/>
     </row>
     <row r="38" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A38" s="6"/>
-      <c r="B38" s="33"/>
+      <c r="B38" s="35"/>
       <c r="C38" s="31"/>
       <c r="D38" s="31"/>
       <c r="E38" s="31"/>
       <c r="F38" s="31"/>
-      <c r="G38" s="36"/>
+      <c r="G38" s="29"/>
       <c r="H38" s="31"/>
       <c r="I38" s="31"/>
-      <c r="J38" s="29"/>
+      <c r="J38" s="33"/>
       <c r="K38" s="6"/>
       <c r="N38" t="s">
         <v>92</v>
@@ -1756,46 +2660,46 @@
     </row>
     <row r="53" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A53" s="6"/>
-      <c r="B53" s="32" t="s">
+      <c r="B53" s="34" t="s">
         <v>0</v>
       </c>
-      <c r="C53" s="30" t="s">
+      <c r="C53" s="36" t="s">
         <v>14</v>
       </c>
-      <c r="D53" s="30" t="s">
+      <c r="D53" s="36" t="s">
         <v>13</v>
       </c>
-      <c r="E53" s="30" t="s">
+      <c r="E53" s="36" t="s">
         <v>12</v>
       </c>
-      <c r="F53" s="34" t="s">
+      <c r="F53" s="30" t="s">
         <v>1</v>
       </c>
-      <c r="G53" s="35" t="s">
+      <c r="G53" s="28" t="s">
         <v>2</v>
       </c>
-      <c r="H53" s="34" t="s">
+      <c r="H53" s="30" t="s">
         <v>3</v>
       </c>
-      <c r="I53" s="34" t="s">
+      <c r="I53" s="30" t="s">
         <v>4</v>
       </c>
-      <c r="J53" s="28" t="s">
+      <c r="J53" s="32" t="s">
         <v>5</v>
       </c>
       <c r="K53" s="6"/>
     </row>
     <row r="54" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A54" s="6"/>
-      <c r="B54" s="33"/>
+      <c r="B54" s="35"/>
       <c r="C54" s="31"/>
       <c r="D54" s="31"/>
       <c r="E54" s="31"/>
       <c r="F54" s="31"/>
-      <c r="G54" s="36"/>
+      <c r="G54" s="29"/>
       <c r="H54" s="31"/>
       <c r="I54" s="31"/>
-      <c r="J54" s="29"/>
+      <c r="J54" s="33"/>
       <c r="K54" s="6"/>
     </row>
     <row r="55" spans="1:18" ht="24" customHeight="1" x14ac:dyDescent="0.2">
@@ -2013,46 +2917,46 @@
     </row>
     <row r="70" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A70" s="6"/>
-      <c r="B70" s="32" t="s">
+      <c r="B70" s="34" t="s">
         <v>0</v>
       </c>
-      <c r="C70" s="30" t="s">
+      <c r="C70" s="36" t="s">
         <v>14</v>
       </c>
-      <c r="D70" s="30" t="s">
+      <c r="D70" s="36" t="s">
         <v>13</v>
       </c>
-      <c r="E70" s="30" t="s">
+      <c r="E70" s="36" t="s">
         <v>12</v>
       </c>
-      <c r="F70" s="34" t="s">
+      <c r="F70" s="30" t="s">
         <v>1</v>
       </c>
-      <c r="G70" s="35" t="s">
+      <c r="G70" s="28" t="s">
         <v>2</v>
       </c>
-      <c r="H70" s="34" t="s">
+      <c r="H70" s="30" t="s">
         <v>3</v>
       </c>
-      <c r="I70" s="34" t="s">
+      <c r="I70" s="30" t="s">
         <v>4</v>
       </c>
-      <c r="J70" s="28" t="s">
+      <c r="J70" s="32" t="s">
         <v>5</v>
       </c>
       <c r="K70" s="6"/>
     </row>
     <row r="71" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A71" s="6"/>
-      <c r="B71" s="33"/>
+      <c r="B71" s="35"/>
       <c r="C71" s="31"/>
       <c r="D71" s="31"/>
       <c r="E71" s="31"/>
       <c r="F71" s="31"/>
-      <c r="G71" s="36"/>
+      <c r="G71" s="29"/>
       <c r="H71" s="31"/>
       <c r="I71" s="31"/>
-      <c r="J71" s="29"/>
+      <c r="J71" s="33"/>
       <c r="K71" s="6"/>
     </row>
     <row r="72" spans="1:17" ht="23" customHeight="1" x14ac:dyDescent="0.2">
@@ -2256,46 +3160,46 @@
     </row>
     <row r="87" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A87" s="6"/>
-      <c r="B87" s="32" t="s">
+      <c r="B87" s="34" t="s">
         <v>0</v>
       </c>
-      <c r="C87" s="30" t="s">
+      <c r="C87" s="36" t="s">
         <v>14</v>
       </c>
-      <c r="D87" s="30" t="s">
+      <c r="D87" s="36" t="s">
         <v>13</v>
       </c>
-      <c r="E87" s="30" t="s">
+      <c r="E87" s="36" t="s">
         <v>12</v>
       </c>
-      <c r="F87" s="34" t="s">
+      <c r="F87" s="30" t="s">
         <v>1</v>
       </c>
-      <c r="G87" s="35" t="s">
+      <c r="G87" s="28" t="s">
         <v>2</v>
       </c>
-      <c r="H87" s="34" t="s">
+      <c r="H87" s="30" t="s">
         <v>3</v>
       </c>
-      <c r="I87" s="34" t="s">
+      <c r="I87" s="30" t="s">
         <v>4</v>
       </c>
-      <c r="J87" s="28" t="s">
+      <c r="J87" s="32" t="s">
         <v>5</v>
       </c>
       <c r="K87" s="6"/>
     </row>
     <row r="88" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A88" s="6"/>
-      <c r="B88" s="33"/>
+      <c r="B88" s="35"/>
       <c r="C88" s="31"/>
       <c r="D88" s="31"/>
       <c r="E88" s="31"/>
       <c r="F88" s="31"/>
-      <c r="G88" s="36"/>
+      <c r="G88" s="29"/>
       <c r="H88" s="31"/>
       <c r="I88" s="31"/>
-      <c r="J88" s="29"/>
+      <c r="J88" s="33"/>
       <c r="K88" s="6"/>
     </row>
     <row r="89" spans="1:21" ht="23" customHeight="1" x14ac:dyDescent="0.2">
@@ -2518,46 +3422,46 @@
     </row>
     <row r="104" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A104" s="6"/>
-      <c r="B104" s="32" t="s">
+      <c r="B104" s="34" t="s">
         <v>0</v>
       </c>
-      <c r="C104" s="30" t="s">
+      <c r="C104" s="36" t="s">
         <v>14</v>
       </c>
-      <c r="D104" s="30" t="s">
+      <c r="D104" s="36" t="s">
         <v>13</v>
       </c>
-      <c r="E104" s="30" t="s">
+      <c r="E104" s="36" t="s">
         <v>12</v>
       </c>
-      <c r="F104" s="34" t="s">
+      <c r="F104" s="30" t="s">
         <v>1</v>
       </c>
-      <c r="G104" s="35" t="s">
+      <c r="G104" s="28" t="s">
         <v>2</v>
       </c>
-      <c r="H104" s="34" t="s">
+      <c r="H104" s="30" t="s">
         <v>3</v>
       </c>
-      <c r="I104" s="34" t="s">
+      <c r="I104" s="30" t="s">
         <v>4</v>
       </c>
-      <c r="J104" s="28" t="s">
+      <c r="J104" s="32" t="s">
         <v>5</v>
       </c>
       <c r="K104" s="6"/>
     </row>
     <row r="105" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A105" s="6"/>
-      <c r="B105" s="33"/>
+      <c r="B105" s="35"/>
       <c r="C105" s="31"/>
       <c r="D105" s="31"/>
       <c r="E105" s="31"/>
       <c r="F105" s="31"/>
-      <c r="G105" s="36"/>
+      <c r="G105" s="29"/>
       <c r="H105" s="31"/>
       <c r="I105" s="31"/>
-      <c r="J105" s="29"/>
+      <c r="J105" s="33"/>
       <c r="K105" s="6"/>
     </row>
     <row r="106" spans="1:17" ht="24" customHeight="1" x14ac:dyDescent="0.2">
@@ -2764,46 +3668,46 @@
     </row>
     <row r="120" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A120" s="6"/>
-      <c r="B120" s="32" t="s">
+      <c r="B120" s="34" t="s">
         <v>0</v>
       </c>
-      <c r="C120" s="30" t="s">
+      <c r="C120" s="36" t="s">
         <v>14</v>
       </c>
-      <c r="D120" s="30" t="s">
+      <c r="D120" s="36" t="s">
         <v>13</v>
       </c>
-      <c r="E120" s="30" t="s">
+      <c r="E120" s="36" t="s">
         <v>12</v>
       </c>
-      <c r="F120" s="34" t="s">
+      <c r="F120" s="30" t="s">
         <v>1</v>
       </c>
-      <c r="G120" s="35" t="s">
+      <c r="G120" s="28" t="s">
         <v>2</v>
       </c>
-      <c r="H120" s="34" t="s">
+      <c r="H120" s="30" t="s">
         <v>3</v>
       </c>
-      <c r="I120" s="34" t="s">
+      <c r="I120" s="30" t="s">
         <v>4</v>
       </c>
-      <c r="J120" s="28" t="s">
+      <c r="J120" s="32" t="s">
         <v>5</v>
       </c>
       <c r="K120" s="6"/>
     </row>
     <row r="121" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A121" s="6"/>
-      <c r="B121" s="33"/>
+      <c r="B121" s="35"/>
       <c r="C121" s="31"/>
       <c r="D121" s="31"/>
       <c r="E121" s="31"/>
       <c r="F121" s="31"/>
-      <c r="G121" s="36"/>
+      <c r="G121" s="29"/>
       <c r="H121" s="31"/>
       <c r="I121" s="31"/>
-      <c r="J121" s="29"/>
+      <c r="J121" s="33"/>
       <c r="K121" s="6"/>
     </row>
     <row r="122" spans="1:14" ht="25" customHeight="1" x14ac:dyDescent="0.2">
@@ -3019,30 +3923,38 @@
     </row>
   </sheetData>
   <mergeCells count="72">
-    <mergeCell ref="G37:G38"/>
-    <mergeCell ref="H37:H38"/>
-    <mergeCell ref="I37:I38"/>
-    <mergeCell ref="J37:J38"/>
-    <mergeCell ref="B53:B54"/>
-    <mergeCell ref="C53:C54"/>
-    <mergeCell ref="D53:D54"/>
-    <mergeCell ref="E53:E54"/>
-    <mergeCell ref="F53:F54"/>
-    <mergeCell ref="G53:G54"/>
-    <mergeCell ref="H53:H54"/>
-    <mergeCell ref="I53:I54"/>
-    <mergeCell ref="J53:J54"/>
-    <mergeCell ref="E37:E38"/>
-    <mergeCell ref="F37:F38"/>
-    <mergeCell ref="H120:H121"/>
-    <mergeCell ref="I120:I121"/>
-    <mergeCell ref="J120:J121"/>
-    <mergeCell ref="B120:B121"/>
-    <mergeCell ref="C120:C121"/>
-    <mergeCell ref="D120:D121"/>
-    <mergeCell ref="E120:E121"/>
-    <mergeCell ref="F120:F121"/>
-    <mergeCell ref="G120:G121"/>
+    <mergeCell ref="J4:J5"/>
+    <mergeCell ref="C4:C5"/>
+    <mergeCell ref="D4:D5"/>
+    <mergeCell ref="B21:B22"/>
+    <mergeCell ref="C21:C22"/>
+    <mergeCell ref="D21:D22"/>
+    <mergeCell ref="E21:E22"/>
+    <mergeCell ref="F21:F22"/>
+    <mergeCell ref="G21:G22"/>
+    <mergeCell ref="B4:B5"/>
+    <mergeCell ref="E4:E5"/>
+    <mergeCell ref="F4:F5"/>
+    <mergeCell ref="G4:G5"/>
+    <mergeCell ref="H4:H5"/>
+    <mergeCell ref="I4:I5"/>
+    <mergeCell ref="H21:H22"/>
+    <mergeCell ref="E104:E105"/>
+    <mergeCell ref="F104:F105"/>
+    <mergeCell ref="I21:I22"/>
+    <mergeCell ref="J21:J22"/>
+    <mergeCell ref="B70:B71"/>
+    <mergeCell ref="C70:C71"/>
+    <mergeCell ref="D70:D71"/>
+    <mergeCell ref="E70:E71"/>
+    <mergeCell ref="F70:F71"/>
+    <mergeCell ref="G70:G71"/>
+    <mergeCell ref="H70:H71"/>
+    <mergeCell ref="I70:I71"/>
+    <mergeCell ref="J70:J71"/>
+    <mergeCell ref="B37:B38"/>
+    <mergeCell ref="C37:C38"/>
+    <mergeCell ref="D37:D38"/>
     <mergeCell ref="G104:G105"/>
     <mergeCell ref="H104:H105"/>
     <mergeCell ref="I104:I105"/>
@@ -3059,39 +3971,415 @@
     <mergeCell ref="B104:B105"/>
     <mergeCell ref="C104:C105"/>
     <mergeCell ref="D104:D105"/>
-    <mergeCell ref="E104:E105"/>
-    <mergeCell ref="F104:F105"/>
-    <mergeCell ref="I21:I22"/>
-    <mergeCell ref="J21:J22"/>
-    <mergeCell ref="B70:B71"/>
-    <mergeCell ref="C70:C71"/>
-    <mergeCell ref="D70:D71"/>
-    <mergeCell ref="E70:E71"/>
-    <mergeCell ref="F70:F71"/>
-    <mergeCell ref="G70:G71"/>
-    <mergeCell ref="H70:H71"/>
-    <mergeCell ref="I70:I71"/>
-    <mergeCell ref="J70:J71"/>
-    <mergeCell ref="B37:B38"/>
-    <mergeCell ref="C37:C38"/>
-    <mergeCell ref="D37:D38"/>
-    <mergeCell ref="J4:J5"/>
-    <mergeCell ref="C4:C5"/>
-    <mergeCell ref="D4:D5"/>
-    <mergeCell ref="B21:B22"/>
-    <mergeCell ref="C21:C22"/>
-    <mergeCell ref="D21:D22"/>
-    <mergeCell ref="E21:E22"/>
-    <mergeCell ref="F21:F22"/>
-    <mergeCell ref="G21:G22"/>
-    <mergeCell ref="B4:B5"/>
-    <mergeCell ref="E4:E5"/>
-    <mergeCell ref="F4:F5"/>
-    <mergeCell ref="G4:G5"/>
-    <mergeCell ref="H4:H5"/>
-    <mergeCell ref="I4:I5"/>
-    <mergeCell ref="H21:H22"/>
+    <mergeCell ref="H120:H121"/>
+    <mergeCell ref="I120:I121"/>
+    <mergeCell ref="J120:J121"/>
+    <mergeCell ref="B120:B121"/>
+    <mergeCell ref="C120:C121"/>
+    <mergeCell ref="D120:D121"/>
+    <mergeCell ref="E120:E121"/>
+    <mergeCell ref="F120:F121"/>
+    <mergeCell ref="G120:G121"/>
+    <mergeCell ref="G37:G38"/>
+    <mergeCell ref="H37:H38"/>
+    <mergeCell ref="I37:I38"/>
+    <mergeCell ref="J37:J38"/>
+    <mergeCell ref="B53:B54"/>
+    <mergeCell ref="C53:C54"/>
+    <mergeCell ref="D53:D54"/>
+    <mergeCell ref="E53:E54"/>
+    <mergeCell ref="F53:F54"/>
+    <mergeCell ref="G53:G54"/>
+    <mergeCell ref="H53:H54"/>
+    <mergeCell ref="I53:I54"/>
+    <mergeCell ref="J53:J54"/>
+    <mergeCell ref="E37:E38"/>
+    <mergeCell ref="F37:F38"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EBD7C3A7-B8E1-A24A-8DCC-865932D639EE}">
+  <dimension ref="A3:Q10"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="11" max="11" width="22.83203125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="3" spans="1:17" s="37" customFormat="1" ht="51" x14ac:dyDescent="0.2">
+      <c r="B3" s="38" t="s">
+        <v>124</v>
+      </c>
+      <c r="C3" s="38" t="s">
+        <v>125</v>
+      </c>
+      <c r="D3" s="38" t="s">
+        <v>126</v>
+      </c>
+      <c r="E3" s="38" t="s">
+        <v>127</v>
+      </c>
+      <c r="F3" s="38" t="s">
+        <v>128</v>
+      </c>
+      <c r="G3" s="38" t="s">
+        <v>129</v>
+      </c>
+      <c r="H3" s="38" t="s">
+        <v>130</v>
+      </c>
+      <c r="I3" s="38" t="s">
+        <v>131</v>
+      </c>
+      <c r="J3" s="38" t="s">
+        <v>132</v>
+      </c>
+      <c r="K3" s="38" t="s">
+        <v>133</v>
+      </c>
+      <c r="L3" s="38" t="s">
+        <v>134</v>
+      </c>
+      <c r="M3" s="38" t="s">
+        <v>135</v>
+      </c>
+      <c r="N3" s="38" t="s">
+        <v>136</v>
+      </c>
+      <c r="O3" s="38" t="s">
+        <v>137</v>
+      </c>
+      <c r="P3" s="38" t="s">
+        <v>138</v>
+      </c>
+      <c r="Q3" s="38" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="5" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A5">
+        <v>3</v>
+      </c>
+      <c r="B5" t="s">
+        <v>108</v>
+      </c>
+      <c r="C5" t="s">
+        <v>19</v>
+      </c>
+      <c r="D5" t="s">
+        <v>109</v>
+      </c>
+      <c r="E5" t="s">
+        <v>110</v>
+      </c>
+      <c r="F5" t="s">
+        <v>111</v>
+      </c>
+      <c r="G5">
+        <v>9.4758856249973107</v>
+      </c>
+      <c r="H5" t="s">
+        <v>112</v>
+      </c>
+      <c r="I5" t="s">
+        <v>113</v>
+      </c>
+      <c r="J5" t="s">
+        <v>114</v>
+      </c>
+      <c r="K5" t="s">
+        <v>115</v>
+      </c>
+      <c r="L5">
+        <v>6.2812416988890604E-2</v>
+      </c>
+      <c r="M5">
+        <v>0.56937799043062198</v>
+      </c>
+      <c r="N5">
+        <v>0.84210526315789402</v>
+      </c>
+      <c r="O5">
+        <v>0.84210526315789402</v>
+      </c>
+      <c r="P5">
+        <v>0.84210526315789402</v>
+      </c>
+      <c r="Q5">
+        <v>0.72727272727272696</v>
+      </c>
+    </row>
+    <row r="6" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A6">
+        <v>0</v>
+      </c>
+      <c r="B6" t="s">
+        <v>108</v>
+      </c>
+      <c r="C6" t="s">
+        <v>19</v>
+      </c>
+      <c r="D6" t="s">
+        <v>140</v>
+      </c>
+      <c r="E6" t="s">
+        <v>141</v>
+      </c>
+      <c r="F6" t="s">
+        <v>111</v>
+      </c>
+      <c r="G6">
+        <v>7.8896797919878701</v>
+      </c>
+      <c r="H6" t="s">
+        <v>142</v>
+      </c>
+      <c r="I6" t="s">
+        <v>143</v>
+      </c>
+      <c r="J6" t="s">
+        <v>114</v>
+      </c>
+      <c r="K6" t="s">
+        <v>115</v>
+      </c>
+      <c r="L6">
+        <v>5.3513499995460699E-2</v>
+      </c>
+      <c r="M6">
+        <v>0.43808582711518002</v>
+      </c>
+      <c r="N6">
+        <v>1</v>
+      </c>
+      <c r="O6">
+        <v>0.70370370370370305</v>
+      </c>
+      <c r="P6">
+        <v>0.82608695652173902</v>
+      </c>
+      <c r="Q6">
+        <v>0.27272727272727199</v>
+      </c>
+    </row>
+    <row r="7" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A7">
+        <v>11</v>
+      </c>
+      <c r="B7" t="s">
+        <v>108</v>
+      </c>
+      <c r="C7" t="s">
+        <v>19</v>
+      </c>
+      <c r="D7" t="s">
+        <v>116</v>
+      </c>
+      <c r="E7" t="s">
+        <v>117</v>
+      </c>
+      <c r="F7" t="s">
+        <v>118</v>
+      </c>
+      <c r="G7">
+        <v>30.170736916013901</v>
+      </c>
+      <c r="H7" t="s">
+        <v>119</v>
+      </c>
+      <c r="I7" t="s">
+        <v>113</v>
+      </c>
+      <c r="J7" t="s">
+        <v>120</v>
+      </c>
+      <c r="K7" t="s">
+        <v>121</v>
+      </c>
+      <c r="L7">
+        <v>6.3386250112671396E-3</v>
+      </c>
+      <c r="M7">
+        <v>0.39795757799683601</v>
+      </c>
+      <c r="N7">
+        <v>0.89473684210526305</v>
+      </c>
+      <c r="O7">
+        <v>0.73913043478260798</v>
+      </c>
+      <c r="P7">
+        <v>0.80952380952380898</v>
+      </c>
+      <c r="Q7">
+        <v>0.45454545454545398</v>
+      </c>
+    </row>
+    <row r="8" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A8">
+        <v>17</v>
+      </c>
+      <c r="B8" t="s">
+        <v>108</v>
+      </c>
+      <c r="C8" t="s">
+        <v>19</v>
+      </c>
+      <c r="D8" t="s">
+        <v>144</v>
+      </c>
+      <c r="E8" t="s">
+        <v>141</v>
+      </c>
+      <c r="F8" t="s">
+        <v>145</v>
+      </c>
+      <c r="G8">
+        <v>2.5997217079857302</v>
+      </c>
+      <c r="H8" t="s">
+        <v>146</v>
+      </c>
+      <c r="I8" t="s">
+        <v>143</v>
+      </c>
+      <c r="J8" t="s">
+        <v>120</v>
+      </c>
+      <c r="K8" t="s">
+        <v>121</v>
+      </c>
+      <c r="L8">
+        <v>3.7227499997243198E-3</v>
+      </c>
+      <c r="M8">
+        <v>0.20751433915982201</v>
+      </c>
+      <c r="N8">
+        <v>0.94736842105263097</v>
+      </c>
+      <c r="O8">
+        <v>0.66666666666666596</v>
+      </c>
+      <c r="P8">
+        <v>0.78260869565217395</v>
+      </c>
+      <c r="Q8">
+        <v>0.18181818181818099</v>
+      </c>
+    </row>
+    <row r="9" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A9">
+        <v>4</v>
+      </c>
+      <c r="B9" t="s">
+        <v>108</v>
+      </c>
+      <c r="C9" t="s">
+        <v>19</v>
+      </c>
+      <c r="D9" t="s">
+        <v>109</v>
+      </c>
+      <c r="E9" t="s">
+        <v>110</v>
+      </c>
+      <c r="F9" t="s">
+        <v>111</v>
+      </c>
+      <c r="G9">
+        <v>68.521575916005503</v>
+      </c>
+      <c r="H9" t="s">
+        <v>122</v>
+      </c>
+      <c r="I9" t="s">
+        <v>113</v>
+      </c>
+      <c r="J9" t="s">
+        <v>114</v>
+      </c>
+      <c r="K9" t="s">
+        <v>123</v>
+      </c>
+      <c r="L9">
+        <v>1.2745333020575299E-2</v>
+      </c>
+      <c r="M9">
+        <v>0.29578954665861401</v>
+      </c>
+      <c r="N9">
+        <v>0.57894736842105199</v>
+      </c>
+      <c r="O9">
+        <v>0.78571428571428503</v>
+      </c>
+      <c r="P9">
+        <v>0.66666666666666596</v>
+      </c>
+      <c r="Q9">
+        <v>0.72727272727272696</v>
+      </c>
+    </row>
+    <row r="10" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A10">
+        <v>1</v>
+      </c>
+      <c r="B10" t="s">
+        <v>108</v>
+      </c>
+      <c r="C10" t="s">
+        <v>19</v>
+      </c>
+      <c r="D10" t="s">
+        <v>140</v>
+      </c>
+      <c r="E10" t="s">
+        <v>141</v>
+      </c>
+      <c r="F10" t="s">
+        <v>111</v>
+      </c>
+      <c r="G10">
+        <v>4.7643824999977298</v>
+      </c>
+      <c r="H10" t="s">
+        <v>147</v>
+      </c>
+      <c r="I10" t="s">
+        <v>143</v>
+      </c>
+      <c r="J10" t="s">
+        <v>114</v>
+      </c>
+      <c r="K10" t="s">
+        <v>123</v>
+      </c>
+      <c r="L10">
+        <v>8.1201082997722496E-2</v>
+      </c>
+      <c r="M10">
+        <v>0.23441336786115</v>
+      </c>
+      <c r="N10">
+        <v>0.84210526315789402</v>
+      </c>
+      <c r="O10">
+        <v>0.69565217391304301</v>
+      </c>
+      <c r="P10">
+        <v>0.76190476190476097</v>
+      </c>
+      <c r="Q10">
+        <v>0.36363636363636298</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>